<commit_message>
ihr scaling 0.5 to 4
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App_2.xlsx
+++ b/Template_CoMoCOVID-19App_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD30A7C6-FCCA-2245-9E42-0F6734044706}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C05F841-3462-0C40-B103-9D85A891F9EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27100" windowHeight="17540" tabRatio="648" activeTab="7" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
@@ -5589,7 +5589,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>